<commit_message>
Commit test cases related to Sighup
</commit_message>
<xml_diff>
--- a/TrinityTwoProj/Data.xlsx
+++ b/TrinityTwoProj/Data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="50">
   <si>
     <t>LoginTest</t>
   </si>
@@ -98,6 +98,78 @@
   </si>
   <si>
     <t>abc@gmail.com</t>
+  </si>
+  <si>
+    <t>trinityTwoLogin</t>
+  </si>
+  <si>
+    <t>SignupEmail</t>
+  </si>
+  <si>
+    <t>SignupPhoneNumber</t>
+  </si>
+  <si>
+    <t>a@b.com</t>
+  </si>
+  <si>
+    <t>trinityTwoSignup</t>
+  </si>
+  <si>
+    <t>x@y.com</t>
+  </si>
+  <si>
+    <t>trinityTwoLoginPageTitle</t>
+  </si>
+  <si>
+    <t>Sign up to your account</t>
+  </si>
+  <si>
+    <t>trinityTwoSignupPageHeader</t>
+  </si>
+  <si>
+    <t>SignupHeader</t>
+  </si>
+  <si>
+    <t>TrinityTwoSignupValidateEmail</t>
+  </si>
+  <si>
+    <t>TCName</t>
+  </si>
+  <si>
+    <t>TRINITYTWO_LOGIN_PAGE_TITLE</t>
+  </si>
+  <si>
+    <t>TRINITYTWO_SIGNUP_PAGE_HEADER</t>
+  </si>
+  <si>
+    <t>signupToAccount</t>
+  </si>
+  <si>
+    <t>SIGNUP_TO_ACCOUNT</t>
+  </si>
+  <si>
+    <t>SIGNUP_VALIDATE_EMAIL_NEGATIVE</t>
+  </si>
+  <si>
+    <t>Email is required.</t>
+  </si>
+  <si>
+    <t>EmailErrorMessage</t>
+  </si>
+  <si>
+    <t>trinityTwosignupValidateEmailNegative</t>
+  </si>
+  <si>
+    <t>trinityTwosignupValidatePhoneNumberNegative</t>
+  </si>
+  <si>
+    <t>SIGNUP_VALIDATE_PHONENUMBER_NEGATIVE</t>
+  </si>
+  <si>
+    <t>PhoneErrorMessage</t>
+  </si>
+  <si>
+    <t>Phone number is required.</t>
   </si>
 </sst>
 </file>
@@ -121,7 +193,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -152,6 +224,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -166,7 +244,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -174,6 +252,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -455,15 +534,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="45.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -503,6 +582,70 @@
         <v>21</v>
       </c>
       <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" t="s">
         <v>7</v>
       </c>
     </row>
@@ -513,18 +656,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="45.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
   </cols>
@@ -692,6 +835,306 @@
       <c r="E16" t="s">
         <v>23</v>
       </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="C23" s="2"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30">
+        <v>1312432342</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" s="2"/>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F33" s="3"/>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34">
+        <v>4563432342</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" s="2"/>
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F37" s="3"/>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" t="s">
+        <v>47</v>
+      </c>
+      <c r="D38" t="s">
+        <v>29</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="E39" s="2"/>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="E40" s="2"/>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" t="s">
+        <v>29</v>
+      </c>
+      <c r="D43">
+        <v>1312432342</v>
+      </c>
+      <c r="E43" s="2"/>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" t="s">
+        <v>31</v>
+      </c>
+      <c r="D47">
+        <v>1312432342</v>
+      </c>
+      <c r="E47" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
pusing the latest changes
</commit_message>
<xml_diff>
--- a/TrinityTwoProj/Data.xlsx
+++ b/TrinityTwoProj/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440"/>
   </bookViews>
   <sheets>
     <sheet name="Test Status" sheetId="2" r:id="rId1"/>
@@ -118,15 +118,9 @@
     <t>x@y.com</t>
   </si>
   <si>
-    <t>trinityTwoLoginPageTitle</t>
-  </si>
-  <si>
     <t>Sign up to your account</t>
   </si>
   <si>
-    <t>trinityTwoSignupPageHeader</t>
-  </si>
-  <si>
     <t>SignupHeader</t>
   </si>
   <si>
@@ -157,19 +151,25 @@
     <t>EmailErrorMessage</t>
   </si>
   <si>
-    <t>trinityTwosignupValidateEmailNegative</t>
-  </si>
-  <si>
-    <t>trinityTwosignupValidatePhoneNumberNegative</t>
-  </si>
-  <si>
     <t>SIGNUP_VALIDATE_PHONENUMBER_NEGATIVE</t>
   </si>
   <si>
     <t>PhoneErrorMessage</t>
   </si>
   <si>
-    <t>Phone number is required.</t>
+    <t>trinityTwo_Signup_Page_Header</t>
+  </si>
+  <si>
+    <t>trinityTwo_Login_Page_Title</t>
+  </si>
+  <si>
+    <t>trinityTwo_Signup_ValidateEmail_Negative</t>
+  </si>
+  <si>
+    <t>trinityTwo_Signup_ValidatePhoneNumber_Negative</t>
+  </si>
+  <si>
+    <t>Phone is required.</t>
   </si>
 </sst>
 </file>
@@ -526,7 +526,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -536,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -587,7 +587,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -595,7 +595,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -619,7 +619,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -627,7 +627,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
@@ -635,7 +635,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -643,7 +643,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
@@ -658,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -852,7 +852,7 @@
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="1" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -863,7 +863,7 @@
         <v>3</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
@@ -877,7 +877,7 @@
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E22" s="2"/>
     </row>
@@ -887,7 +887,7 @@
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="1" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C24" s="2"/>
       <c r="E24" s="2"/>
@@ -900,10 +900,10 @@
         <v>3</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -916,10 +916,10 @@
         <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E26" s="2"/>
     </row>
@@ -928,7 +928,7 @@
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C28" s="2"/>
       <c r="E28" s="2"/>
@@ -941,7 +941,7 @@
         <v>3</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>27</v>
@@ -959,7 +959,7 @@
         <v>8</v>
       </c>
       <c r="C30" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D30" t="s">
         <v>29</v>
@@ -973,7 +973,7 @@
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C32" s="2"/>
       <c r="E32" s="2"/>
@@ -986,13 +986,13 @@
         <v>3</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F33" s="3"/>
     </row>
@@ -1004,13 +1004,13 @@
         <v>8</v>
       </c>
       <c r="C34" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D34">
         <v>4563432342</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1018,7 +1018,7 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C36" s="2"/>
       <c r="E36" s="2"/>
@@ -1031,13 +1031,13 @@
         <v>3</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F37" s="3"/>
     </row>
@@ -1049,7 +1049,7 @@
         <v>8</v>
       </c>
       <c r="C38" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D38" t="s">
         <v>29</v>

</xml_diff>